<commit_message>
- just forced a change to commit
</commit_message>
<xml_diff>
--- a/excel-app/DataBase.xlsx
+++ b/excel-app/DataBase.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lfs\IOGC\RoyaltyModule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\$temp\git\python-playground\excel-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="6045" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -11277,7 +11277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -11429,8 +11429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Continue Sask Oil Calcs
</commit_message>
<xml_diff>
--- a/excel-app/DataBase.xlsx
+++ b/excel-app/DataBase.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\$temp\git\python-playground\excel-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\python-playground\excel-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="152">
   <si>
     <t>Lease Type</t>
   </si>
@@ -456,9 +456,6 @@
     <t>SWNEW_K</t>
   </si>
   <si>
-    <t>WSNEW_X</t>
-  </si>
-  <si>
     <t>O4T_K</t>
   </si>
   <si>
@@ -478,6 +475,15 @@
   </si>
   <si>
     <t>bad one</t>
+  </si>
+  <si>
+    <t>Bad Tax Class</t>
+  </si>
+  <si>
+    <t>SWNEW_X</t>
+  </si>
+  <si>
+    <t>Bad One</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1280,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N16" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1343,7 +1351,7 @@
         <v>141</v>
       </c>
       <c r="V1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="W1" t="s">
         <v>134</v>
@@ -1352,22 +1360,22 @@
         <v>135</v>
       </c>
       <c r="Y1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z1" t="s">
         <v>143</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>144</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>145</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>146</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>147</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>148</v>
       </c>
       <c r="AE1" t="s">
         <v>137</v>
@@ -11275,10 +11283,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11363,6 +11371,9 @@
       <c r="B6" t="s">
         <v>92</v>
       </c>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -11417,7 +11428,231 @@
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -11427,10 +11662,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12199,6 +12434,652 @@
         <v>84</v>
       </c>
       <c r="L20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2015</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="16">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
+      <c r="I21">
+        <v>100</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2015</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>100</v>
+      </c>
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2015</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23">
+        <v>100</v>
+      </c>
+      <c r="I23">
+        <v>100</v>
+      </c>
+      <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23" t="s">
+        <v>84</v>
+      </c>
+      <c r="L23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2015</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24">
+        <v>100</v>
+      </c>
+      <c r="I24">
+        <v>100</v>
+      </c>
+      <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24" t="s">
+        <v>84</v>
+      </c>
+      <c r="L24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2015</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25">
+        <v>13</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25">
+        <v>100</v>
+      </c>
+      <c r="I25">
+        <v>100</v>
+      </c>
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25" t="s">
+        <v>84</v>
+      </c>
+      <c r="L25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2015</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26">
+        <v>14</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26">
+        <v>100</v>
+      </c>
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2015</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27">
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27">
+        <v>100</v>
+      </c>
+      <c r="I27">
+        <v>100</v>
+      </c>
+      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27" t="s">
+        <v>84</v>
+      </c>
+      <c r="L27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2015</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28">
+        <v>100</v>
+      </c>
+      <c r="I28">
+        <v>100</v>
+      </c>
+      <c r="J28">
+        <v>100</v>
+      </c>
+      <c r="K28" t="s">
+        <v>84</v>
+      </c>
+      <c r="L28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2015</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29">
+        <v>100</v>
+      </c>
+      <c r="I29">
+        <v>100</v>
+      </c>
+      <c r="J29">
+        <v>100</v>
+      </c>
+      <c r="K29" t="s">
+        <v>84</v>
+      </c>
+      <c r="L29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2015</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30">
+        <v>18</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30">
+        <v>100</v>
+      </c>
+      <c r="I30">
+        <v>100</v>
+      </c>
+      <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30" t="s">
+        <v>84</v>
+      </c>
+      <c r="L30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2015</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31">
+        <v>100</v>
+      </c>
+      <c r="I31">
+        <v>100</v>
+      </c>
+      <c r="J31">
+        <v>100</v>
+      </c>
+      <c r="K31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2015</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32">
+        <v>100</v>
+      </c>
+      <c r="I32">
+        <v>100</v>
+      </c>
+      <c r="J32">
+        <v>100</v>
+      </c>
+      <c r="K32" t="s">
+        <v>84</v>
+      </c>
+      <c r="L32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2015</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33">
+        <v>21</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33">
+        <v>100</v>
+      </c>
+      <c r="I33">
+        <v>100</v>
+      </c>
+      <c r="J33">
+        <v>100</v>
+      </c>
+      <c r="K33" t="s">
+        <v>84</v>
+      </c>
+      <c r="L33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2015</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34">
+        <v>22</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34">
+        <v>100</v>
+      </c>
+      <c r="I34">
+        <v>100</v>
+      </c>
+      <c r="J34">
+        <v>100</v>
+      </c>
+      <c r="K34" t="s">
+        <v>84</v>
+      </c>
+      <c r="L34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2015</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35">
+        <v>23</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35">
+        <v>100</v>
+      </c>
+      <c r="I35">
+        <v>100</v>
+      </c>
+      <c r="J35">
+        <v>100</v>
+      </c>
+      <c r="K35" t="s">
+        <v>84</v>
+      </c>
+      <c r="L35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2015</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36">
+        <v>24</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36">
+        <v>100</v>
+      </c>
+      <c r="I36">
+        <v>100</v>
+      </c>
+      <c r="J36">
+        <v>100</v>
+      </c>
+      <c r="K36" t="s">
+        <v>84</v>
+      </c>
+      <c r="L36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2015</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37">
+        <v>25</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37">
+        <v>100</v>
+      </c>
+      <c r="I37">
+        <v>100</v>
+      </c>
+      <c r="J37">
+        <v>100</v>
+      </c>
+      <c r="K37" t="s">
+        <v>84</v>
+      </c>
+      <c r="L37" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Sask SRC code and testing
</commit_message>
<xml_diff>
--- a/excel-app/DataBase.xlsx
+++ b/excel-app/DataBase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView topLeftCell="N16" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11285,7 +11285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:A26"/>
     </sheetView>
   </sheetViews>
@@ -11664,7 +11664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Update src just started
</commit_message>
<xml_diff>
--- a/excel-app/DataBase.xlsx
+++ b/excel-app/DataBase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="154">
   <si>
     <t>Lease Type</t>
   </si>
@@ -484,6 +484,12 @@
   </si>
   <si>
     <t>Bad One</t>
+  </si>
+  <si>
+    <t>CrownInterest</t>
+  </si>
+  <si>
+    <t>SRC</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -6061,20 +6067,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1001"/>
+  <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -6088,13 +6097,16 @@
         <v>71</v>
       </c>
       <c r="E1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6107,14 +6119,17 @@
       <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>46</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6127,14 +6142,17 @@
       <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6147,14 +6165,17 @@
       <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>46</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6167,14 +6188,17 @@
       <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>46</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6187,59 +6211,62 @@
       <c r="D6" t="s">
         <v>44</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
         <v>46</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11283,10 +11310,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11294,7 +11321,7 @@
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -11307,8 +11334,11 @@
       <c r="D1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11322,7 +11352,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11336,7 +11366,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11350,7 +11380,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11364,7 +11394,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11375,7 +11405,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11389,7 +11419,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11403,7 +11433,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11417,7 +11447,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11431,7 +11461,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11445,7 +11475,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11459,7 +11489,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11473,7 +11503,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11487,7 +11517,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11501,7 +11531,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11664,8 +11694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Rename Fetch to DataBase - Add worksheet generation
</commit_message>
<xml_diff>
--- a/excel-app/DataBase.xlsx
+++ b/excel-app/DataBase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="152">
   <si>
     <t>Lease Type</t>
   </si>
@@ -473,6 +473,18 @@
   </si>
   <si>
     <t>PTF</t>
+  </si>
+  <si>
+    <t>UWI</t>
+  </si>
+  <si>
+    <t>100 14 36 085 17 W3 00</t>
+  </si>
+  <si>
+    <t>SalesPrice</t>
+  </si>
+  <si>
+    <t>TransPrice</t>
   </si>
 </sst>
 </file>
@@ -11344,609 +11356,687 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>87</v>
       </c>
       <c r="B1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>144</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>147</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>90</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>95</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>112</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
         <v>79</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>92</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>48</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
         <v>79</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>93</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>48</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" t="s">
         <v>83</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>140</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
         <v>79</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>92</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>95</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
         <v>79</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>92</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>112</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" t="s">
         <v>79</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>92</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>48</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" t="s">
         <v>79</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>92</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>139</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" t="s">
         <v>79</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>91</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>95</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" t="s">
         <v>79</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>91</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>112</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" t="s">
         <v>79</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>91</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>48</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" t="s">
         <v>79</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>91</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>139</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" t="s">
         <v>79</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>90</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>95</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>90</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>112</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" t="s">
         <v>79</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>48</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" t="s">
         <v>79</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>90</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>139</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" t="s">
         <v>79</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>93</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>95</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" t="s">
         <v>79</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>93</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>112</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" t="s">
         <v>79</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>93</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>48</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" t="s">
         <v>79</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>93</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>139</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
         <v>79</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>142</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>95</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" t="s">
         <v>79</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>142</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>112</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" t="s">
         <v>79</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>142</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>48</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" t="s">
         <v>79</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>142</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>139</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>1</v>
       </c>
     </row>
@@ -11957,10 +12047,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="L3" sqref="L3:L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11972,7 +12062,7 @@
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -12004,10 +12094,16 @@
         <v>60</v>
       </c>
       <c r="K1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12041,8 +12137,14 @@
       <c r="K2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12076,8 +12178,14 @@
       <c r="K3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12111,8 +12219,14 @@
       <c r="K4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12146,8 +12260,14 @@
       <c r="K5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12181,8 +12301,14 @@
       <c r="K6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12216,8 +12342,14 @@
       <c r="K7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -12251,8 +12383,14 @@
       <c r="K8">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12286,8 +12424,14 @@
       <c r="K9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -12321,8 +12465,14 @@
       <c r="K10">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -12356,8 +12506,14 @@
       <c r="K11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -12391,8 +12547,14 @@
       <c r="K12">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -12426,8 +12588,14 @@
       <c r="K13">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -12461,8 +12629,14 @@
       <c r="K14">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -12496,8 +12670,14 @@
       <c r="K15">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -12531,8 +12711,14 @@
       <c r="K16">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -12566,8 +12752,14 @@
       <c r="K17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -12601,8 +12793,14 @@
       <c r="K18">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -12636,8 +12834,14 @@
       <c r="K19">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -12671,8 +12875,14 @@
       <c r="K20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -12706,8 +12916,14 @@
       <c r="K21">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -12741,8 +12957,14 @@
       <c r="K22">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -12776,8 +12998,14 @@
       <c r="K23">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -12811,8 +13039,14 @@
       <c r="K24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -12846,8 +13080,14 @@
       <c r="K25">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -12881,8 +13121,14 @@
       <c r="K26">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -12916,8 +13162,14 @@
       <c r="K27">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -12951,8 +13203,14 @@
       <c r="K28">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -12986,8 +13244,14 @@
       <c r="K29">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -13021,8 +13285,14 @@
       <c r="K30">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -13056,8 +13326,14 @@
       <c r="K31">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -13091,8 +13367,14 @@
       <c r="K32">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -13126,8 +13408,14 @@
       <c r="K33">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -13161,8 +13449,14 @@
       <c r="K34">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -13196,8 +13490,14 @@
       <c r="K35">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -13231,8 +13531,14 @@
       <c r="K36">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -13264,6 +13570,12 @@
         <v>100</v>
       </c>
       <c r="K37">
+        <v>100</v>
+      </c>
+      <c r="L37">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M37">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Continue Royalty Report
</commit_message>
<xml_diff>
--- a/excel-app/DataBase.xlsx
+++ b/excel-app/DataBase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="155">
   <si>
     <t>Lease Type</t>
   </si>
@@ -223,9 +223,6 @@
     <t>NGX</t>
   </si>
   <si>
-    <t>ProvincialCrownMultiplier</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -485,6 +482,18 @@
   </si>
   <si>
     <t>TransPrice</t>
+  </si>
+  <si>
+    <t>TransportationDeducted</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>ProcessingDeducted</t>
+  </si>
+  <si>
+    <t>CrownMultiplier</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1058,8 +1067,8 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>365/12</f>
-        <v>30.416666666666668</v>
+        <f>20.9*2.2</f>
+        <v>45.980000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,19 +1317,19 @@
         <v>58</v>
       </c>
       <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
         <v>67</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1340,105 +1349,105 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" t="s">
-        <v>99</v>
-      </c>
       <c r="G1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" t="s">
         <v>114</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>115</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>116</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>117</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>118</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>119</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>120</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>121</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>122</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>123</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" t="s">
+        <v>130</v>
+      </c>
+      <c r="U1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W1" t="s">
         <v>124</v>
       </c>
-      <c r="R1" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" t="s">
-        <v>130</v>
-      </c>
-      <c r="T1" t="s">
-        <v>131</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y1" t="s">
         <v>132</v>
       </c>
-      <c r="V1" t="s">
-        <v>141</v>
-      </c>
-      <c r="W1" t="s">
-        <v>125</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF1" t="s">
         <v>126</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -1536,7 +1545,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -1634,7 +1643,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -1732,7 +1741,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -1830,7 +1839,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1928,7 +1937,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2026,7 +2035,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2124,7 +2133,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2222,7 +2231,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2320,7 +2329,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11">
         <v>12</v>
@@ -2418,7 +2427,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2516,7 +2525,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -2614,7 +2623,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -2712,7 +2721,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -2810,7 +2819,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -2908,7 +2917,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -3006,7 +3015,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -3104,7 +3113,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3202,7 +3211,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -3300,7 +3309,7 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -3398,7 +3407,7 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3496,7 +3505,7 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23">
         <v>12</v>
@@ -3594,7 +3603,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24">
         <v>11</v>
@@ -3692,7 +3701,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B25">
         <v>10</v>
@@ -3790,7 +3799,7 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26">
         <v>9</v>
@@ -3888,7 +3897,7 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3986,7 +3995,7 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28">
         <v>7</v>
@@ -4084,7 +4093,7 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29">
         <v>6</v>
@@ -4182,7 +4191,7 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -4280,7 +4289,7 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -4378,7 +4387,7 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -4476,7 +4485,7 @@
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -4574,7 +4583,7 @@
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4672,7 +4681,7 @@
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35">
         <v>12</v>
@@ -4770,7 +4779,7 @@
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36">
         <v>11</v>
@@ -4868,7 +4877,7 @@
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37">
         <v>10</v>
@@ -4966,7 +4975,7 @@
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38">
         <v>9</v>
@@ -5064,7 +5073,7 @@
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -5162,7 +5171,7 @@
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40">
         <v>7</v>
@@ -5260,7 +5269,7 @@
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41">
         <v>6</v>
@@ -5358,7 +5367,7 @@
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42">
         <v>5</v>
@@ -5456,7 +5465,7 @@
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5554,7 +5563,7 @@
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -5652,7 +5661,7 @@
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -5750,7 +5759,7 @@
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -5848,7 +5857,7 @@
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B47">
         <v>12</v>
@@ -5946,7 +5955,7 @@
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B48">
         <v>11</v>
@@ -6065,7 +6074,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
@@ -6113,10 +6122,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1001"/>
+  <dimension ref="A1:I1001"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6129,7 +6138,7 @@
     <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -6140,19 +6149,25 @@
         <v>53</v>
       </c>
       <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
       <c r="G1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="H1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6160,10 +6175,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -6172,10 +6187,16 @@
         <v>46</v>
       </c>
       <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6183,10 +6204,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6195,10 +6216,16 @@
         <v>46</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6206,7 +6233,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>44</v>
@@ -6220,8 +6247,14 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6229,7 +6262,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
@@ -6243,8 +6276,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6252,7 +6291,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -6266,53 +6305,59 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>152</v>
+      </c>
+      <c r="I6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11286,10 +11331,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>123</v>
@@ -11303,10 +11348,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>123</v>
@@ -11320,10 +11365,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4">
         <v>123</v>
@@ -11337,10 +11382,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5">
         <v>123</v>
@@ -11369,28 +11414,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" t="s">
         <v>144</v>
-      </c>
-      <c r="G1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -11398,16 +11443,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -11424,16 +11469,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -11450,13 +11495,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
@@ -11476,13 +11521,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
         <v>48</v>
@@ -11502,13 +11547,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -11525,16 +11570,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -11551,16 +11596,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -11577,13 +11622,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
@@ -11603,16 +11648,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -11629,16 +11674,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -11655,16 +11700,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -11681,13 +11726,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
         <v>48</v>
@@ -11707,16 +11752,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -11733,16 +11778,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -11759,16 +11804,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -11785,13 +11830,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
         <v>48</v>
@@ -11811,16 +11856,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -11837,16 +11882,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -11863,16 +11908,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -11889,13 +11934,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
         <v>48</v>
@@ -11915,16 +11960,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -11941,16 +11986,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -11967,16 +12012,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -11993,13 +12038,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E25" t="s">
         <v>48</v>
@@ -12019,16 +12064,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -12049,8 +12094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12064,7 +12109,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
@@ -12079,10 +12124,10 @@
         <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s">
         <v>58</v>
@@ -12094,10 +12139,10 @@
         <v>60</v>
       </c>
       <c r="K1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L1" t="s">
         <v>150</v>
-      </c>
-      <c r="L1" t="s">
-        <v>151</v>
       </c>
       <c r="M1" t="s">
         <v>61</v>
@@ -12117,7 +12162,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="16">
         <v>1</v>
@@ -12126,7 +12171,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -12135,13 +12180,13 @@
         <v>100</v>
       </c>
       <c r="K2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L2">
         <v>2.2000000000000002</v>
       </c>
       <c r="M2">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -12158,7 +12203,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" s="16">
         <v>2</v>
@@ -12167,7 +12212,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3">
         <v>100</v>
@@ -12176,13 +12221,13 @@
         <v>100</v>
       </c>
       <c r="K3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L3">
         <v>2.2000000000000002</v>
       </c>
       <c r="M3">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -12199,7 +12244,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="16">
         <v>3</v>
@@ -12208,7 +12253,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I4">
         <v>100</v>
@@ -12217,13 +12262,13 @@
         <v>100</v>
       </c>
       <c r="K4">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L4">
         <v>2.2000000000000002</v>
       </c>
       <c r="M4">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -12240,7 +12285,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="16">
         <v>4</v>
@@ -12249,7 +12294,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5">
         <v>100</v>
@@ -12258,13 +12303,13 @@
         <v>100</v>
       </c>
       <c r="K5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L5">
         <v>2.2000000000000002</v>
       </c>
       <c r="M5">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -12281,7 +12326,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="16">
         <v>1</v>
@@ -12290,7 +12335,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I6">
         <v>100</v>
@@ -12299,13 +12344,13 @@
         <v>100</v>
       </c>
       <c r="K6">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L6">
         <v>2.2000000000000002</v>
       </c>
       <c r="M6">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -12322,7 +12367,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="16">
         <v>2</v>
@@ -12331,7 +12376,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7">
         <v>100</v>
@@ -12340,13 +12385,13 @@
         <v>100</v>
       </c>
       <c r="K7">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L7">
         <v>2.2000000000000002</v>
       </c>
       <c r="M7">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -12363,7 +12408,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="16">
         <v>3</v>
@@ -12372,7 +12417,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8">
         <v>100</v>
@@ -12381,13 +12426,13 @@
         <v>100</v>
       </c>
       <c r="K8">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L8">
         <v>2.2000000000000002</v>
       </c>
       <c r="M8">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -12404,7 +12449,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="16">
         <v>4</v>
@@ -12413,7 +12458,7 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9">
         <v>100</v>
@@ -12422,13 +12467,13 @@
         <v>100</v>
       </c>
       <c r="K9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L9">
         <v>2.2000000000000002</v>
       </c>
       <c r="M9">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -12445,7 +12490,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" s="16">
         <v>1</v>
@@ -12454,7 +12499,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10">
         <v>100</v>
@@ -12463,13 +12508,13 @@
         <v>100</v>
       </c>
       <c r="K10">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L10">
         <v>2.2000000000000002</v>
       </c>
       <c r="M10">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -12486,7 +12531,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" s="16">
         <v>2</v>
@@ -12495,7 +12540,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I11">
         <v>100</v>
@@ -12504,13 +12549,13 @@
         <v>100</v>
       </c>
       <c r="K11">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L11">
         <v>2.2000000000000002</v>
       </c>
       <c r="M11">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -12527,7 +12572,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="16">
         <v>6</v>
@@ -12536,7 +12581,7 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12">
         <v>10</v>
@@ -12545,13 +12590,13 @@
         <v>100</v>
       </c>
       <c r="K12">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L12">
         <v>2.2000000000000002</v>
       </c>
       <c r="M12">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -12568,7 +12613,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" s="16">
         <v>6</v>
@@ -12577,7 +12622,7 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I13">
         <v>100</v>
@@ -12586,13 +12631,13 @@
         <v>100</v>
       </c>
       <c r="K13">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L13">
         <v>2.2000000000000002</v>
       </c>
       <c r="M13">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -12609,7 +12654,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" s="16">
         <v>7</v>
@@ -12618,7 +12663,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I14">
         <v>100</v>
@@ -12627,13 +12672,13 @@
         <v>100</v>
       </c>
       <c r="K14">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L14">
         <v>2.2000000000000002</v>
       </c>
       <c r="M14">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -12650,7 +12695,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="16">
         <v>8</v>
@@ -12659,7 +12704,7 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I15">
         <v>100</v>
@@ -12668,13 +12713,13 @@
         <v>100</v>
       </c>
       <c r="K15">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L15">
         <v>2.2000000000000002</v>
       </c>
       <c r="M15">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -12691,7 +12736,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" s="16">
         <v>9</v>
@@ -12700,7 +12745,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I16">
         <v>100</v>
@@ -12709,13 +12754,13 @@
         <v>100</v>
       </c>
       <c r="K16">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L16">
         <v>2.2000000000000002</v>
       </c>
       <c r="M16">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -12732,7 +12777,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F17" s="16">
         <v>6</v>
@@ -12741,7 +12786,7 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I17">
         <v>200</v>
@@ -12750,13 +12795,13 @@
         <v>100</v>
       </c>
       <c r="K17">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L17">
         <v>2.2000000000000002</v>
       </c>
       <c r="M17">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -12773,7 +12818,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F18" s="16">
         <v>7</v>
@@ -12782,7 +12827,7 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I18">
         <v>200</v>
@@ -12791,13 +12836,13 @@
         <v>100</v>
       </c>
       <c r="K18">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L18">
         <v>2.2000000000000002</v>
       </c>
       <c r="M18">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -12814,7 +12859,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" s="16">
         <v>8</v>
@@ -12823,7 +12868,7 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I19">
         <v>200</v>
@@ -12832,13 +12877,13 @@
         <v>100</v>
       </c>
       <c r="K19">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L19">
         <v>2.2000000000000002</v>
       </c>
       <c r="M19">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -12855,7 +12900,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="16">
         <v>9</v>
@@ -12864,7 +12909,7 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I20">
         <v>200</v>
@@ -12873,13 +12918,13 @@
         <v>100</v>
       </c>
       <c r="K20">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L20">
         <v>2.2000000000000002</v>
       </c>
       <c r="M20">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -12896,7 +12941,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F21" s="16">
         <v>10</v>
@@ -12905,7 +12950,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I21">
         <v>100</v>
@@ -12914,13 +12959,13 @@
         <v>100</v>
       </c>
       <c r="K21">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L21">
         <v>2.2000000000000002</v>
       </c>
       <c r="M21">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -12937,7 +12982,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -12946,7 +12991,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I22">
         <v>100</v>
@@ -12955,13 +13000,13 @@
         <v>100</v>
       </c>
       <c r="K22">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L22">
         <v>2.2000000000000002</v>
       </c>
       <c r="M22">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -12978,7 +13023,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -12987,7 +13032,7 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I23">
         <v>100</v>
@@ -12996,13 +13041,13 @@
         <v>100</v>
       </c>
       <c r="K23">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L23">
         <v>2.2000000000000002</v>
       </c>
       <c r="M23">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -13019,7 +13064,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -13028,7 +13073,7 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I24">
         <v>100</v>
@@ -13037,13 +13082,13 @@
         <v>100</v>
       </c>
       <c r="K24">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L24">
         <v>2.2000000000000002</v>
       </c>
       <c r="M24">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -13060,7 +13105,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F25">
         <v>13</v>
@@ -13069,7 +13114,7 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I25">
         <v>100</v>
@@ -13078,13 +13123,13 @@
         <v>100</v>
       </c>
       <c r="K25">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L25">
         <v>2.2000000000000002</v>
       </c>
       <c r="M25">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -13101,7 +13146,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F26">
         <v>14</v>
@@ -13110,7 +13155,7 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I26">
         <v>100</v>
@@ -13119,13 +13164,13 @@
         <v>100</v>
       </c>
       <c r="K26">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L26">
         <v>2.2000000000000002</v>
       </c>
       <c r="M26">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -13142,7 +13187,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F27">
         <v>15</v>
@@ -13151,7 +13196,7 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I27">
         <v>100</v>
@@ -13160,13 +13205,13 @@
         <v>100</v>
       </c>
       <c r="K27">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L27">
         <v>2.2000000000000002</v>
       </c>
       <c r="M27">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -13183,7 +13228,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F28">
         <v>16</v>
@@ -13192,7 +13237,7 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I28">
         <v>100</v>
@@ -13201,13 +13246,13 @@
         <v>100</v>
       </c>
       <c r="K28">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L28">
         <v>2.2000000000000002</v>
       </c>
       <c r="M28">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -13224,7 +13269,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F29">
         <v>17</v>
@@ -13233,7 +13278,7 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I29">
         <v>100</v>
@@ -13242,13 +13287,13 @@
         <v>100</v>
       </c>
       <c r="K29">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L29">
         <v>2.2000000000000002</v>
       </c>
       <c r="M29">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -13265,7 +13310,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F30">
         <v>18</v>
@@ -13274,7 +13319,7 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I30">
         <v>100</v>
@@ -13283,13 +13328,13 @@
         <v>100</v>
       </c>
       <c r="K30">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L30">
         <v>2.2000000000000002</v>
       </c>
       <c r="M30">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -13306,7 +13351,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31">
         <v>19</v>
@@ -13315,7 +13360,7 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I31">
         <v>100</v>
@@ -13324,13 +13369,13 @@
         <v>100</v>
       </c>
       <c r="K31">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L31">
         <v>2.2000000000000002</v>
       </c>
       <c r="M31">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -13347,7 +13392,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F32">
         <v>20</v>
@@ -13356,7 +13401,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I32">
         <v>100</v>
@@ -13365,13 +13410,13 @@
         <v>100</v>
       </c>
       <c r="K32">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L32">
         <v>2.2000000000000002</v>
       </c>
       <c r="M32">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -13388,7 +13433,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F33">
         <v>21</v>
@@ -13397,7 +13442,7 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I33">
         <v>100</v>
@@ -13406,13 +13451,13 @@
         <v>100</v>
       </c>
       <c r="K33">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L33">
         <v>2.2000000000000002</v>
       </c>
       <c r="M33">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -13429,7 +13474,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F34">
         <v>22</v>
@@ -13438,7 +13483,7 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I34">
         <v>100</v>
@@ -13447,13 +13492,13 @@
         <v>100</v>
       </c>
       <c r="K34">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L34">
         <v>2.2000000000000002</v>
       </c>
       <c r="M34">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -13470,7 +13515,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F35">
         <v>23</v>
@@ -13479,7 +13524,7 @@
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I35">
         <v>100</v>
@@ -13488,13 +13533,13 @@
         <v>100</v>
       </c>
       <c r="K35">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L35">
         <v>2.2000000000000002</v>
       </c>
       <c r="M35">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -13511,7 +13556,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F36">
         <v>24</v>
@@ -13520,7 +13565,7 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I36">
         <v>100</v>
@@ -13529,13 +13574,13 @@
         <v>100</v>
       </c>
       <c r="K36">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L36">
         <v>2.2000000000000002</v>
       </c>
       <c r="M36">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -13552,7 +13597,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F37">
         <v>25</v>
@@ -13561,7 +13606,7 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I37">
         <v>100</v>
@@ -13570,13 +13615,13 @@
         <v>100</v>
       </c>
       <c r="K37">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L37">
         <v>2.2000000000000002</v>
       </c>
       <c r="M37">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -13596,7 +13641,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
@@ -13611,10 +13656,10 @@
         <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s">
         <v>58</v>
@@ -13643,7 +13688,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="16">
         <v>6</v>
@@ -13652,7 +13697,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -13687,13 +13732,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -13701,7 +13746,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2">
         <v>0.25</v>

</xml_diff>

<commit_message>
- Update based on round 2 of reviews. Add the concept of Valuation Method, Add the concept of deductions, improve the display of factors
</commit_message>
<xml_diff>
--- a/excel-app/DataBase.xlsx
+++ b/excel-app/DataBase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="170">
   <si>
     <t>Lease Type</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Descriptor</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>WellType</t>
   </si>
   <si>
-    <t>TaxClassification</t>
-  </si>
-  <si>
     <t>New Oil</t>
   </si>
   <si>
@@ -342,9 +336,6 @@
     <t>Southwest</t>
   </si>
   <si>
-    <t>ProductClassification</t>
-  </si>
-  <si>
     <t>H4T_C</t>
   </si>
   <si>
@@ -438,9 +429,6 @@
     <t>Row</t>
   </si>
   <si>
-    <t>PTF</t>
-  </si>
-  <si>
     <t>UWI</t>
   </si>
   <si>
@@ -450,9 +438,6 @@
     <t>TransPrice</t>
   </si>
   <si>
-    <t>TransportationDeducted</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -514,6 +499,45 @@
   </si>
   <si>
     <t>Lessor</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>RoyaltyClassification</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>SaskOilVal</t>
+  </si>
+  <si>
+    <t>SaskWellHead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sask Well Head Price as defined in Sask Regulations. The price is net of trucking and processing. </t>
+  </si>
+  <si>
+    <t>Actual Sales Price. Does not deduct trucking or processing</t>
+  </si>
+  <si>
+    <t>ActSales</t>
+  </si>
+  <si>
+    <t>ProcessingRate</t>
+  </si>
+  <si>
+    <t>ValuationMethod</t>
+  </si>
+  <si>
+    <t>TruckingDeducted</t>
   </si>
 </sst>
 </file>
@@ -646,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -691,6 +715,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,7 +1082,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,8 +1121,8 @@
         <v>219.000001</v>
       </c>
       <c r="D5">
-        <f>25.02/100*25*219.000001</f>
-        <v>1369.8450062549998</v>
+        <f>26.85 *  1.1 *    100 *  0.95 * 223.370366/100</f>
+        <v>6267.3815718195001</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1338,102 +1363,102 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
       <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>106</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>107</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>108</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>109</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>110</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>111</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>112</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R1" t="s">
+        <v>118</v>
+      </c>
+      <c r="S1" t="s">
+        <v>119</v>
+      </c>
+      <c r="T1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" t="s">
         <v>113</v>
       </c>
-      <c r="O1" t="s">
+      <c r="W1" t="s">
         <v>114</v>
       </c>
-      <c r="P1" t="s">
+      <c r="X1" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE1" t="s">
         <v>115</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R1" t="s">
-        <v>121</v>
-      </c>
-      <c r="S1" t="s">
-        <v>122</v>
-      </c>
-      <c r="T1" t="s">
-        <v>123</v>
-      </c>
-      <c r="U1" t="s">
-        <v>132</v>
-      </c>
-      <c r="V1" t="s">
-        <v>116</v>
-      </c>
-      <c r="W1" t="s">
-        <v>117</v>
-      </c>
-      <c r="X1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2">
         <v>201509</v>
@@ -1528,7 +1553,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>201508</v>
@@ -1623,7 +1648,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4">
         <v>201507</v>
@@ -1718,7 +1743,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5">
         <v>201506</v>
@@ -1813,7 +1838,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6">
         <v>201505</v>
@@ -1908,7 +1933,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>201504</v>
@@ -2003,7 +2028,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8">
         <v>201503</v>
@@ -2098,7 +2123,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B9">
         <v>201502</v>
@@ -2193,7 +2218,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10">
         <v>201501</v>
@@ -2288,7 +2313,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11">
         <v>201412</v>
@@ -2383,7 +2408,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B12">
         <v>201411</v>
@@ -2478,7 +2503,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B13">
         <v>201410</v>
@@ -2573,7 +2598,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14">
         <v>201409</v>
@@ -2668,7 +2693,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>201408</v>
@@ -2763,7 +2788,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B16">
         <v>201407</v>
@@ -2858,7 +2883,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B17">
         <v>201406</v>
@@ -2953,7 +2978,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18">
         <v>201405</v>
@@ -3048,7 +3073,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B19">
         <v>201404</v>
@@ -3143,7 +3168,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B20">
         <v>201403</v>
@@ -3238,7 +3263,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B21">
         <v>201402</v>
@@ -3333,7 +3358,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B22">
         <v>201401</v>
@@ -3428,7 +3453,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23">
         <v>201312</v>
@@ -3523,7 +3548,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B24">
         <v>201311</v>
@@ -3618,7 +3643,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B25">
         <v>201310</v>
@@ -3713,7 +3738,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B26">
         <v>201309</v>
@@ -3808,7 +3833,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B27">
         <v>201308</v>
@@ -3903,7 +3928,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B28">
         <v>201307</v>
@@ -3998,7 +4023,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B29">
         <v>201306</v>
@@ -4093,7 +4118,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B30">
         <v>201305</v>
@@ -4188,7 +4213,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B31">
         <v>201304</v>
@@ -4283,7 +4308,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B32">
         <v>201303</v>
@@ -4378,7 +4403,7 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B33">
         <v>201302</v>
@@ -4473,7 +4498,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B34">
         <v>201301</v>
@@ -4568,7 +4593,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B35">
         <v>201212</v>
@@ -4663,7 +4688,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B36">
         <v>201211</v>
@@ -4758,7 +4783,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B37">
         <v>201210</v>
@@ -4853,7 +4878,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38">
         <v>201209</v>
@@ -4948,7 +4973,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39">
         <v>201208</v>
@@ -5043,7 +5068,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B40">
         <v>201207</v>
@@ -5138,7 +5163,7 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B41">
         <v>201206</v>
@@ -5233,7 +5258,7 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B42">
         <v>201205</v>
@@ -5328,7 +5353,7 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B43">
         <v>201204</v>
@@ -5423,7 +5448,7 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B44">
         <v>201203</v>
@@ -5518,7 +5543,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B45">
         <v>201202</v>
@@ -5613,7 +5638,7 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B46">
         <v>201201</v>
@@ -5708,7 +5733,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B47">
         <v>201112</v>
@@ -5803,7 +5828,7 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48">
         <v>201111</v>
@@ -5903,10 +5928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5917,47 +5942,37 @@
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>162</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -5967,10 +5982,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5981,40 +5996,44 @@
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
-        <v>67</v>
-      </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G1" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="H1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -6025,19 +6044,25 @@
       <c r="E2">
         <v>1.2</v>
       </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
       <c r="G2" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
@@ -6048,19 +6073,22 @@
       <c r="E3">
         <v>1.1000000000000001</v>
       </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="H3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
@@ -6069,21 +6097,21 @@
         <v>46</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="I4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -6092,21 +6120,24 @@
         <v>46</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G5" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="H5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
@@ -6115,13 +6146,10 @@
         <v>46</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="G6" t="s">
-        <v>141</v>
-      </c>
-      <c r="H6" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -6133,8 +6161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6147,24 +6175,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>123</v>
@@ -6175,10 +6203,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>123</v>
@@ -6189,10 +6217,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>123</v>
@@ -6203,10 +6231,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5">
         <v>123</v>
@@ -6225,46 +6253,47 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>149</v>
-      </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>104</v>
+        <v>158</v>
       </c>
       <c r="G1" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="H1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I1" t="s">
-        <v>72</v>
+        <v>131</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6272,27 +6301,27 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="17">
         <v>0.25</v>
       </c>
     </row>
@@ -6301,27 +6330,27 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="17">
         <v>0.95</v>
       </c>
     </row>
@@ -6330,27 +6359,27 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="F4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" t="s">
         <v>48</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6359,27 +6388,27 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
         <v>48</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6388,24 +6417,24 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" t="s">
+        <v>128</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6414,27 +6443,27 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="G7" t="s">
+        <v>84</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6443,27 +6472,27 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="G8" t="s">
+        <v>101</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6472,27 +6501,27 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="F9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" t="s">
         <v>48</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6501,27 +6530,27 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>127</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6530,27 +6559,27 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="F11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="G11" t="s">
+        <v>84</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6559,27 +6588,27 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="F12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="G12" t="s">
+        <v>101</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6588,27 +6617,27 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E13" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="F13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" t="s">
         <v>48</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6617,27 +6646,27 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E14" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
+        <v>127</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6646,27 +6675,27 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="G15" t="s">
+        <v>84</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6675,27 +6704,27 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
+        <v>101</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6704,27 +6733,27 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="F17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
         <v>48</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6733,27 +6762,27 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E18" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="G18" t="s">
+        <v>127</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6762,27 +6791,27 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" t="s">
         <v>84</v>
-      </c>
-      <c r="F19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6791,27 +6820,27 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E20" t="s">
-        <v>84</v>
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>101</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6820,27 +6849,27 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="F21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" t="s">
         <v>48</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6849,27 +6878,27 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="F22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="G22" t="s">
+        <v>127</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6878,27 +6907,27 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E23" t="s">
-        <v>133</v>
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="F23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
+        <v>130</v>
+      </c>
+      <c r="G23" t="s">
+        <v>84</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6907,27 +6936,27 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" t="s">
-        <v>133</v>
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
+        <v>130</v>
+      </c>
+      <c r="G24" t="s">
+        <v>101</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6936,27 +6965,27 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" t="s">
-        <v>133</v>
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="F25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" t="s">
         <v>48</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="17">
         <v>1</v>
       </c>
     </row>
@@ -6965,41 +6994,42 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E26" t="s">
-        <v>133</v>
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="F26" t="s">
         <v>130</v>
       </c>
-      <c r="G26">
-        <v>0</v>
+      <c r="G26" t="s">
+        <v>127</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="17">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L3"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7014,50 +7044,53 @@
     <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" t="s">
-        <v>139</v>
-      </c>
       <c r="K1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="L1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="M1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>201509</v>
+      <c r="B2" s="18">
+        <v>42276</v>
       </c>
       <c r="C2">
         <v>201501</v>
@@ -7066,7 +7099,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -7089,13 +7122,16 @@
       <c r="L2">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>201509</v>
+      <c r="B3" s="18">
+        <v>42276</v>
       </c>
       <c r="C3">
         <v>201502</v>
@@ -7104,7 +7140,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -7127,13 +7163,16 @@
       <c r="L3">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>201509</v>
+      <c r="B4" s="18">
+        <v>42276</v>
       </c>
       <c r="C4">
         <v>201503</v>
@@ -7142,7 +7181,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -7165,13 +7204,16 @@
       <c r="L4">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>201509</v>
+      <c r="B5" s="18">
+        <v>42276</v>
       </c>
       <c r="C5">
         <v>201504</v>
@@ -7180,7 +7222,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -7203,13 +7245,16 @@
       <c r="L5">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>201509</v>
+      <c r="B6" s="18">
+        <v>42276</v>
       </c>
       <c r="C6">
         <v>201504</v>
@@ -7218,7 +7263,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -7241,13 +7286,16 @@
       <c r="L6">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>201509</v>
+      <c r="B7" s="18">
+        <v>42276</v>
       </c>
       <c r="C7">
         <v>201504</v>
@@ -7256,7 +7304,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -7279,13 +7327,16 @@
       <c r="L7">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>201509</v>
+      <c r="B8" s="18">
+        <v>42276</v>
       </c>
       <c r="C8">
         <v>201504</v>
@@ -7294,7 +7345,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -7317,13 +7368,16 @@
       <c r="L8">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>201509</v>
+      <c r="B9" s="18">
+        <v>42276</v>
       </c>
       <c r="C9">
         <v>201504</v>
@@ -7332,7 +7386,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -7355,13 +7409,16 @@
       <c r="L9">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>201509</v>
+      <c r="B10" s="18">
+        <v>42276</v>
       </c>
       <c r="C10">
         <v>201504</v>
@@ -7370,7 +7427,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -7393,13 +7450,16 @@
       <c r="L10">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>201509</v>
+      <c r="B11" s="18">
+        <v>42276</v>
       </c>
       <c r="C11">
         <v>201503</v>
@@ -7408,7 +7468,7 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -7431,13 +7491,16 @@
       <c r="L11">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>201509</v>
+      <c r="B12" s="18">
+        <v>42276</v>
       </c>
       <c r="C12">
         <v>201503</v>
@@ -7446,7 +7509,7 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -7469,13 +7532,16 @@
       <c r="L12">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>201509</v>
+      <c r="B13" s="18">
+        <v>42276</v>
       </c>
       <c r="C13">
         <v>201503</v>
@@ -7484,7 +7550,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -7507,13 +7573,16 @@
       <c r="L13">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>201509</v>
+      <c r="B14" s="18">
+        <v>42276</v>
       </c>
       <c r="C14">
         <v>201503</v>
@@ -7522,7 +7591,7 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -7545,13 +7614,16 @@
       <c r="L14">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>201509</v>
+      <c r="B15" s="18">
+        <v>42276</v>
       </c>
       <c r="C15">
         <v>201503</v>
@@ -7560,7 +7632,7 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -7583,13 +7655,16 @@
       <c r="L15">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>201509</v>
+      <c r="B16" s="18">
+        <v>42276</v>
       </c>
       <c r="C16">
         <v>201504</v>
@@ -7598,7 +7673,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -7621,13 +7696,16 @@
       <c r="L16">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>201509</v>
+      <c r="B17" s="18">
+        <v>42276</v>
       </c>
       <c r="C17">
         <v>201504</v>
@@ -7636,7 +7714,7 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -7659,13 +7737,16 @@
       <c r="L17">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>201509</v>
+      <c r="B18" s="18">
+        <v>42276</v>
       </c>
       <c r="C18">
         <v>201504</v>
@@ -7674,7 +7755,7 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -7697,13 +7778,16 @@
       <c r="L18">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>201509</v>
+      <c r="B19" s="18">
+        <v>42276</v>
       </c>
       <c r="C19">
         <v>201504</v>
@@ -7712,7 +7796,7 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -7735,13 +7819,16 @@
       <c r="L19">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>201509</v>
+      <c r="B20" s="18">
+        <v>42276</v>
       </c>
       <c r="C20">
         <v>201504</v>
@@ -7750,7 +7837,7 @@
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -7773,13 +7860,16 @@
       <c r="L20">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>201509</v>
+      <c r="B21" s="18">
+        <v>42276</v>
       </c>
       <c r="C21">
         <v>201504</v>
@@ -7788,7 +7878,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F21">
         <v>6</v>
@@ -7811,13 +7901,16 @@
       <c r="L21">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>201509</v>
+      <c r="B22" s="18">
+        <v>42276</v>
       </c>
       <c r="C22">
         <v>201504</v>
@@ -7826,7 +7919,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22">
         <v>7</v>
@@ -7849,13 +7942,16 @@
       <c r="L22">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>201509</v>
+      <c r="B23" s="18">
+        <v>42276</v>
       </c>
       <c r="C23">
         <v>201504</v>
@@ -7864,7 +7960,7 @@
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23">
         <v>8</v>
@@ -7887,13 +7983,16 @@
       <c r="L23">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>201509</v>
+      <c r="B24" s="18">
+        <v>42276</v>
       </c>
       <c r="C24">
         <v>201504</v>
@@ -7902,7 +8001,7 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24">
         <v>11</v>
@@ -7925,13 +8024,16 @@
       <c r="L24">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>201509</v>
+      <c r="B25" s="18">
+        <v>42276</v>
       </c>
       <c r="C25">
         <v>201504</v>
@@ -7940,7 +8042,7 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -7963,13 +8065,16 @@
       <c r="L25">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>201509</v>
+      <c r="B26" s="18">
+        <v>42276</v>
       </c>
       <c r="C26">
         <v>201504</v>
@@ -7978,7 +8083,7 @@
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -8001,13 +8106,16 @@
       <c r="L26">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>201509</v>
+      <c r="B27" s="18">
+        <v>42276</v>
       </c>
       <c r="C27">
         <v>201504</v>
@@ -8016,7 +8124,7 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -8039,13 +8147,16 @@
       <c r="L27">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28">
-        <v>201509</v>
+      <c r="B28" s="18">
+        <v>42276</v>
       </c>
       <c r="C28">
         <v>201504</v>
@@ -8054,7 +8165,7 @@
         <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28">
         <v>3</v>
@@ -8077,13 +8188,16 @@
       <c r="L28">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>201509</v>
+      <c r="B29" s="18">
+        <v>42276</v>
       </c>
       <c r="C29">
         <v>201504</v>
@@ -8092,7 +8206,7 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29">
         <v>4</v>
@@ -8115,13 +8229,16 @@
       <c r="L29">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>201509</v>
+      <c r="B30" s="18">
+        <v>42276</v>
       </c>
       <c r="C30">
         <v>201504</v>
@@ -8130,7 +8247,7 @@
         <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30">
         <v>5</v>
@@ -8153,13 +8270,16 @@
       <c r="L30">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31">
-        <v>201509</v>
+      <c r="B31" s="18">
+        <v>42276</v>
       </c>
       <c r="C31">
         <v>201504</v>
@@ -8168,7 +8288,7 @@
         <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F31">
         <v>6</v>
@@ -8191,13 +8311,16 @@
       <c r="L31">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>201509</v>
+      <c r="B32" s="18">
+        <v>42276</v>
       </c>
       <c r="C32">
         <v>201504</v>
@@ -8206,7 +8329,7 @@
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32">
         <v>2</v>
@@ -8229,13 +8352,16 @@
       <c r="L32">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33">
-        <v>201509</v>
+      <c r="B33" s="18">
+        <v>42276</v>
       </c>
       <c r="C33">
         <v>201504</v>
@@ -8244,7 +8370,7 @@
         <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F33">
         <v>3</v>
@@ -8267,13 +8393,16 @@
       <c r="L33">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>201509</v>
+      <c r="B34" s="18">
+        <v>42276</v>
       </c>
       <c r="C34">
         <v>201504</v>
@@ -8282,7 +8411,7 @@
         <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34">
         <v>4</v>
@@ -8305,13 +8434,16 @@
       <c r="L34">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35">
-        <v>201509</v>
+      <c r="B35" s="18">
+        <v>42276</v>
       </c>
       <c r="C35">
         <v>201504</v>
@@ -8320,7 +8452,7 @@
         <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F35">
         <v>5</v>
@@ -8343,13 +8475,16 @@
       <c r="L35">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36">
-        <v>201509</v>
+      <c r="B36" s="18">
+        <v>42276</v>
       </c>
       <c r="C36">
         <v>201504</v>
@@ -8358,7 +8493,7 @@
         <v>24</v>
       </c>
       <c r="E36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F36">
         <v>6</v>
@@ -8381,13 +8516,16 @@
       <c r="L36">
         <v>2.1234549999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37">
-        <v>201509</v>
+      <c r="B37" s="18">
+        <v>42276</v>
       </c>
       <c r="C37">
         <v>201504</v>
@@ -8396,7 +8534,7 @@
         <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F37">
         <v>2</v>
@@ -8418,6 +8556,9 @@
       </c>
       <c r="L37">
         <v>2.1234549999999999</v>
+      </c>
+      <c r="M37">
+        <v>0.123455</v>
       </c>
     </row>
   </sheetData>
@@ -8441,13 +8582,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
         <v>71</v>
-      </c>
-      <c r="C1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8455,7 +8596,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>0.25</v>
@@ -8481,10 +8622,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -8514,28 +8655,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Start on Regulation Royalties - Start a better test harness - Start breaking down the big classes
</commit_message>
<xml_diff>
--- a/excel-app/DataBase.xlsx
+++ b/excel-app/DataBase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="179">
   <si>
     <t>Lease Type</t>
   </si>
@@ -538,6 +538,33 @@
   </si>
   <si>
     <t>TruckingDeducted</t>
+  </si>
+  <si>
+    <t>SKProvCrownVar</t>
+  </si>
+  <si>
+    <t>OL-0006</t>
+  </si>
+  <si>
+    <t>Regulation1995</t>
+  </si>
+  <si>
+    <t>CommencementDate</t>
+  </si>
+  <si>
+    <t>ReferencePrice</t>
+  </si>
+  <si>
+    <t>OL-2000</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>(Used for Examples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Sask Oil SKProvCrownVar / SaskWellHead / No Deductions / Fourth Tier </t>
   </si>
 </sst>
 </file>
@@ -5930,7 +5957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5982,9 +6009,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -6039,7 +6066,7 @@
         <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="E2">
         <v>1.2</v>
@@ -6068,7 +6095,7 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="E3">
         <v>1.1000000000000001</v>
@@ -6094,7 +6121,7 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="E4">
         <v>0.9</v>
@@ -6117,7 +6144,7 @@
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="E5">
         <v>1.25</v>
@@ -6143,13 +6170,53 @@
         <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="E6">
         <v>0.85</v>
       </c>
       <c r="G6" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8">
+        <v>1.2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -6159,10 +6226,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6243,6 +6310,48 @@
         <v>2345</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7">
+        <v>123</v>
+      </c>
+      <c r="D7">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8">
+        <v>123</v>
+      </c>
+      <c r="D8">
+        <v>2345</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6250,10 +6359,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6265,9 +6375,10 @@
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -6295,8 +6406,17 @@
       <c r="I1" s="17" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6324,8 +6444,14 @@
       <c r="I2" s="17">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6353,8 +6479,14 @@
       <c r="I3" s="17">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6383,7 +6515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6412,7 +6544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6438,7 +6570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6467,7 +6599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6496,7 +6628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6525,7 +6657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6554,7 +6686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6583,7 +6715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6612,7 +6744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6641,7 +6773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6670,7 +6802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6699,7 +6831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6728,7 +6860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6757,7 +6889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6786,7 +6918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6815,7 +6947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6844,7 +6976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6873,7 +7005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6902,7 +7034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6931,7 +7063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6960,7 +7092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6989,7 +7121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -7016,6 +7148,122 @@
       </c>
       <c r="I26" s="17">
         <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1000</v>
+      </c>
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="I28" s="17">
+        <v>1</v>
+      </c>
+      <c r="J28" s="18">
+        <v>40513</v>
+      </c>
+      <c r="L28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2000</v>
+      </c>
+      <c r="B29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="L29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2001</v>
+      </c>
+      <c r="B30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" s="17">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -7026,11 +7274,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7096,7 +7342,7 @@
         <v>201501</v>
       </c>
       <c r="D2" s="16">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="E2" t="s">
         <v>69</v>
@@ -7105,7 +7351,7 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>100</v>
@@ -7134,16 +7380,16 @@
         <v>42276</v>
       </c>
       <c r="C3">
-        <v>201502</v>
+        <v>201501</v>
       </c>
       <c r="D3" s="16">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="E3" t="s">
         <v>69</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -7175,19 +7421,19 @@
         <v>42276</v>
       </c>
       <c r="C4">
-        <v>201503</v>
+        <v>201501</v>
       </c>
       <c r="D4" s="16">
-        <v>3</v>
+        <v>2000</v>
       </c>
       <c r="E4" t="s">
         <v>69</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -7216,16 +7462,16 @@
         <v>42276</v>
       </c>
       <c r="C5">
-        <v>201504</v>
+        <v>201501</v>
       </c>
       <c r="D5" s="16">
-        <v>4</v>
+        <v>2001</v>
       </c>
       <c r="E5" t="s">
         <v>69</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -7257,13 +7503,13 @@
         <v>42276</v>
       </c>
       <c r="C6">
-        <v>201504</v>
+        <v>201501</v>
       </c>
       <c r="D6" s="16">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -7298,16 +7544,16 @@
         <v>42276</v>
       </c>
       <c r="C7">
-        <v>201504</v>
+        <v>201501</v>
       </c>
       <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7">
         <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
       </c>
       <c r="G7">
         <v>100</v>
@@ -7339,16 +7585,16 @@
         <v>42276</v>
       </c>
       <c r="C8">
-        <v>201504</v>
+        <v>201502</v>
       </c>
       <c r="D8" s="16">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8">
         <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
       </c>
       <c r="G8">
         <v>100</v>
@@ -7380,16 +7626,16 @@
         <v>42276</v>
       </c>
       <c r="C9">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D9" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -7424,13 +7670,13 @@
         <v>201504</v>
       </c>
       <c r="D10" s="16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
         <v>69</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>100</v>
@@ -7462,16 +7708,16 @@
         <v>42276</v>
       </c>
       <c r="C11">
-        <v>201503</v>
+        <v>201504</v>
       </c>
       <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11">
         <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
       </c>
       <c r="G11">
         <v>100</v>
@@ -7503,19 +7749,19 @@
         <v>42276</v>
       </c>
       <c r="C12">
-        <v>201503</v>
+        <v>201504</v>
       </c>
       <c r="D12" s="16">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
       <c r="G12">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H12">
         <v>100</v>
@@ -7544,16 +7790,16 @@
         <v>42276</v>
       </c>
       <c r="C13">
-        <v>201503</v>
+        <v>201504</v>
       </c>
       <c r="D13" s="16">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G13">
         <v>100</v>
@@ -7585,16 +7831,16 @@
         <v>42276</v>
       </c>
       <c r="C14">
-        <v>201503</v>
+        <v>201504</v>
       </c>
       <c r="D14" s="16">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
         <v>69</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>100</v>
@@ -7626,16 +7872,16 @@
         <v>42276</v>
       </c>
       <c r="C15">
-        <v>201503</v>
+        <v>201504</v>
       </c>
       <c r="D15" s="16">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>69</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>100</v>
@@ -7667,16 +7913,16 @@
         <v>42276</v>
       </c>
       <c r="C16">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D16" s="16">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
         <v>69</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>100</v>
@@ -7708,7 +7954,7 @@
         <v>42276</v>
       </c>
       <c r="C17">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D17" s="16">
         <v>6</v>
@@ -7717,10 +7963,10 @@
         <v>69</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="H17">
         <v>100</v>
@@ -7749,19 +7995,19 @@
         <v>42276</v>
       </c>
       <c r="C18">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D18" s="16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
         <v>69</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H18">
         <v>100</v>
@@ -7790,19 +8036,19 @@
         <v>42276</v>
       </c>
       <c r="C19">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D19" s="16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
         <v>69</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>100</v>
@@ -7831,10 +8077,10 @@
         <v>42276</v>
       </c>
       <c r="C20">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D20" s="16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
         <v>69</v>
@@ -7843,7 +8089,7 @@
         <v>3</v>
       </c>
       <c r="G20">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H20">
         <v>100</v>
@@ -7875,13 +8121,13 @@
         <v>201504</v>
       </c>
       <c r="D21" s="16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
         <v>69</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G21">
         <v>100</v>
@@ -7915,17 +8161,17 @@
       <c r="C22">
         <v>201504</v>
       </c>
-      <c r="D22">
-        <v>10</v>
+      <c r="D22" s="16">
+        <v>6</v>
       </c>
       <c r="E22" t="s">
         <v>69</v>
       </c>
       <c r="F22">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H22">
         <v>100</v>
@@ -7956,17 +8202,17 @@
       <c r="C23">
         <v>201504</v>
       </c>
-      <c r="D23">
-        <v>11</v>
+      <c r="D23" s="16">
+        <v>7</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>
       </c>
       <c r="F23">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H23">
         <v>100</v>
@@ -7997,17 +8243,17 @@
       <c r="C24">
         <v>201504</v>
       </c>
-      <c r="D24">
-        <v>12</v>
+      <c r="D24" s="16">
+        <v>8</v>
       </c>
       <c r="E24" t="s">
         <v>69</v>
       </c>
       <c r="F24">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H24">
         <v>100</v>
@@ -8038,17 +8284,17 @@
       <c r="C25">
         <v>201504</v>
       </c>
-      <c r="D25">
-        <v>13</v>
+      <c r="D25" s="16">
+        <v>9</v>
       </c>
       <c r="E25" t="s">
         <v>69</v>
       </c>
       <c r="F25">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H25">
         <v>100</v>
@@ -8079,14 +8325,14 @@
       <c r="C26">
         <v>201504</v>
       </c>
-      <c r="D26">
-        <v>14</v>
+      <c r="D26" s="16">
+        <v>10</v>
       </c>
       <c r="E26" t="s">
         <v>69</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G26">
         <v>100</v>
@@ -8121,13 +8367,13 @@
         <v>201504</v>
       </c>
       <c r="D27">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
         <v>69</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G27">
         <v>100</v>
@@ -8162,13 +8408,13 @@
         <v>201504</v>
       </c>
       <c r="D28">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
         <v>69</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G28">
         <v>100</v>
@@ -8203,13 +8449,13 @@
         <v>201504</v>
       </c>
       <c r="D29">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
         <v>69</v>
       </c>
       <c r="F29">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G29">
         <v>100</v>
@@ -8244,13 +8490,13 @@
         <v>201504</v>
       </c>
       <c r="D30">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E30" t="s">
         <v>69</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G30">
         <v>100</v>
@@ -8285,13 +8531,13 @@
         <v>201504</v>
       </c>
       <c r="D31">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
         <v>69</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>100</v>
@@ -8326,13 +8572,13 @@
         <v>201504</v>
       </c>
       <c r="D32">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s">
         <v>69</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>100</v>
@@ -8367,7 +8613,7 @@
         <v>201504</v>
       </c>
       <c r="D33">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E33" t="s">
         <v>69</v>
@@ -8408,7 +8654,7 @@
         <v>201504</v>
       </c>
       <c r="D34">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
         <v>69</v>
@@ -8449,7 +8695,7 @@
         <v>201504</v>
       </c>
       <c r="D35">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E35" t="s">
         <v>69</v>
@@ -8490,7 +8736,7 @@
         <v>201504</v>
       </c>
       <c r="D36">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E36" t="s">
         <v>69</v>
@@ -8531,7 +8777,7 @@
         <v>201504</v>
       </c>
       <c r="D37">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
         <v>69</v>
@@ -8558,6 +8804,211 @@
         <v>2.1234549999999999</v>
       </c>
       <c r="M37">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="18">
+        <v>42276</v>
+      </c>
+      <c r="C38">
+        <v>201504</v>
+      </c>
+      <c r="D38">
+        <v>21</v>
+      </c>
+      <c r="E38" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+      <c r="H38">
+        <v>100</v>
+      </c>
+      <c r="I38">
+        <v>200</v>
+      </c>
+      <c r="J38">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K38">
+        <v>221.123456</v>
+      </c>
+      <c r="L38">
+        <v>2.1234549999999999</v>
+      </c>
+      <c r="M38">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="18">
+        <v>42276</v>
+      </c>
+      <c r="C39">
+        <v>201504</v>
+      </c>
+      <c r="D39">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39">
+        <v>4</v>
+      </c>
+      <c r="G39">
+        <v>100</v>
+      </c>
+      <c r="H39">
+        <v>100</v>
+      </c>
+      <c r="I39">
+        <v>200</v>
+      </c>
+      <c r="J39">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K39">
+        <v>221.123456</v>
+      </c>
+      <c r="L39">
+        <v>2.1234549999999999</v>
+      </c>
+      <c r="M39">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="18">
+        <v>42276</v>
+      </c>
+      <c r="C40">
+        <v>201504</v>
+      </c>
+      <c r="D40">
+        <v>23</v>
+      </c>
+      <c r="E40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40">
+        <v>5</v>
+      </c>
+      <c r="G40">
+        <v>100</v>
+      </c>
+      <c r="H40">
+        <v>100</v>
+      </c>
+      <c r="I40">
+        <v>200</v>
+      </c>
+      <c r="J40">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K40">
+        <v>221.123456</v>
+      </c>
+      <c r="L40">
+        <v>2.1234549999999999</v>
+      </c>
+      <c r="M40">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="18">
+        <v>42276</v>
+      </c>
+      <c r="C41">
+        <v>201504</v>
+      </c>
+      <c r="D41">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41">
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+      <c r="H41">
+        <v>100</v>
+      </c>
+      <c r="I41">
+        <v>200</v>
+      </c>
+      <c r="J41">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K41">
+        <v>221.123456</v>
+      </c>
+      <c r="L41">
+        <v>2.1234549999999999</v>
+      </c>
+      <c r="M41">
+        <v>0.123455</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="18">
+        <v>42276</v>
+      </c>
+      <c r="C42">
+        <v>201504</v>
+      </c>
+      <c r="D42">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>100</v>
+      </c>
+      <c r="H42">
+        <v>100</v>
+      </c>
+      <c r="I42">
+        <v>200</v>
+      </c>
+      <c r="J42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K42">
+        <v>221.123456</v>
+      </c>
+      <c r="L42">
+        <v>2.1234549999999999</v>
+      </c>
+      <c r="M42">
         <v>0.123455</v>
       </c>
     </row>

</xml_diff>